<commit_message>
labelled more than 50 points
</commit_message>
<xml_diff>
--- a/data/sample/accuracy_assesment/confidence_rating.xlsx
+++ b/data/sample/accuracy_assesment/confidence_rating.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mapping-wetlands\data\sample\accuracy_assesment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Documents\mapping-wetlands\data\sample\accuracy_assesment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE50EF82-B7B5-4C26-B53B-F725B2DAD98C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DB9FB1-33B3-41A9-9100-A87DD6C8632D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15960" yWindow="600" windowWidth="22080" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7740" yWindow="-90" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="9">
   <si>
     <t>id</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>high</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>algae</t>
+  </si>
+  <si>
+    <t>human induced</t>
   </si>
 </sst>
 </file>
@@ -394,8 +403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E205"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,6 +416,9 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
@@ -427,7 +439,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -465,7 +477,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -540,15 +552,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -556,7 +568,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -564,7 +576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -572,7 +584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -580,15 +592,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -596,15 +611,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -612,7 +627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -620,47 +635,53 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -668,7 +689,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -676,7 +697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -684,7 +705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -692,7 +713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -700,7 +721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -708,7 +729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -716,7 +737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -724,15 +745,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -740,15 +764,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -756,7 +780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -764,7 +788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -772,7 +796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -780,7 +804,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -788,7 +812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -796,23 +820,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -820,7 +847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -828,31 +855,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -860,7 +887,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -868,15 +895,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -884,7 +911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -892,7 +919,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -900,7 +927,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -908,15 +935,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1049,7 +1076,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1057,7 +1084,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1097,7 +1124,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1121,7 +1148,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1153,7 +1180,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1209,7 +1236,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -1225,7 +1252,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -1233,7 +1260,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -1265,7 +1292,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -1409,7 +1436,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -1425,7 +1452,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -1436,7 +1463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -1449,7 +1476,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -1457,7 +1484,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -1553,7 +1580,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -1561,7 +1588,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -1569,7 +1596,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -1593,7 +1620,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -1617,7 +1644,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -1705,7 +1732,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -1737,7 +1764,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -1753,7 +1780,7 @@
         <v>167</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -1777,7 +1804,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -1820,7 +1847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
@@ -1828,7 +1855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
@@ -1836,7 +1863,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
@@ -1844,7 +1871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
@@ -1852,7 +1879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
@@ -1860,15 +1887,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
@@ -1876,7 +1903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
@@ -1884,7 +1911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
@@ -1892,7 +1919,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
@@ -1900,7 +1927,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
@@ -1908,7 +1935,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
@@ -1916,15 +1943,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C189" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
@@ -1932,7 +1962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
@@ -1940,7 +1970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
@@ -2001,7 +2031,7 @@
         <v>198</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
@@ -2033,15 +2063,15 @@
         <v>202</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>203</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>